<commit_message>
Updated test outputs after adding a new manifest to the test db sharepoint area for an new test scenario being implemented
</commit_message>
<xml_diff>
--- a/src/apodeixi/knowledge_base/tests_integration/input_data/basic_posting_flows.big_rocks.burnout/brb_opus.big-rocks.journeys.a6i.xlsx
+++ b/src/apodeixi/knowledge_base/tests_integration/input_data/basic_posting_flows.big_rocks.burnout/brb_opus.big-rocks.journeys.a6i.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\knowledge_base\tests_integration\input_data\basic_posting_flows.big_rocks.burnout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A76C4D-536A-4B44-AF5E-A5649A0C8E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2368B84-2C50-42A2-BFB0-264D59408035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,9 +133,6 @@
     <t>Marathon</t>
   </si>
   <si>
-    <t>simple; burnout</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>G2:H8</t>
+  </si>
+  <si>
+    <t>burnout</t>
   </si>
 </sst>
 </file>
@@ -726,7 +726,7 @@
   <dimension ref="B1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -737,7 +737,7 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.45">
@@ -825,7 +825,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
@@ -833,7 +833,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
@@ -841,7 +841,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
@@ -849,7 +849,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
@@ -873,7 +873,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
@@ -881,7 +881,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
@@ -889,7 +889,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
@@ -897,7 +897,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
@@ -905,7 +905,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
@@ -913,7 +913,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
@@ -921,7 +921,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
@@ -929,7 +929,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
@@ -937,11 +937,11 @@
         <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -966,51 +966,51 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="I2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7">
         <v>4050</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="7">
         <v>3584</v>
@@ -1022,17 +1022,17 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="7">
         <v>6600</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="7">
         <v>5207</v>
@@ -1044,17 +1044,17 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7">
         <v>4500</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" s="7">
         <v>5575</v>
@@ -1066,15 +1066,15 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
       <c r="G6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" s="7">
         <v>5800</v>
@@ -1088,13 +1088,13 @@
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" s="7">
         <v>5100</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="7">
         <v>5860</v>
@@ -1108,13 +1108,13 @@
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" s="7">
         <v>5250</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H8" s="7">
         <v>998</v>
@@ -1127,7 +1127,7 @@
     <row r="9" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="7">
@@ -1139,10 +1139,10 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="7">
@@ -1154,7 +1154,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C11" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="8">

</xml_diff>